<commit_message>
Add existing VRES and BESS
</commit_message>
<xml_diff>
--- a/data/Szenario_Trafo_Full/Power_Storage.xlsx
+++ b/data/Szenario_Trafo_Full/Power_Storage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Trafo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Trafo_Full\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE15D91-16A5-4050-982A-453A88035017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056BE0CE-2B08-4686-919B-87E0CCE297AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1875,10 +1875,10 @@
   </sheetPr>
   <dimension ref="B1:AK12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O55" sqref="O55"/>
-      <selection pane="bottomLeft" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2178,7 @@
         <v>51</v>
       </c>
       <c r="E7" s="17">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F7" s="25">
         <v>50</v>
@@ -2206,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="27">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="T7" s="27">
         <v>3821.0756000000001</v>
@@ -2287,7 +2287,7 @@
         <v>1</v>
       </c>
       <c r="S8" s="27">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="T8" s="27">
         <v>3871.0756000000001</v>
@@ -2340,7 +2340,7 @@
         <v>53</v>
       </c>
       <c r="E9" s="17">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="F9" s="25">
         <v>50</v>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="27">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="T9" s="27">
         <v>3921.0756000000001</v>
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="S10" s="27">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="T10" s="27">
         <v>3971.0756000000001</v>
@@ -2532,7 +2532,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="27">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="T11" s="27">
         <v>4000</v>
@@ -2593,9 +2593,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2745,26 +2748,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2788,9 +2780,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>